<commit_message>
Fungsi Download template kegiatan profesi
</commit_message>
<xml_diff>
--- a/public/assets/import-penunjang.xlsx
+++ b/public/assets/import-penunjang.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-v8.0\htdocs\laravel-9\kemendagri-damkar-boot\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\magang\abbauf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2672AF-1221-4764-BF32-BA99B755B6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77169E68-A3F5-4FCF-AD46-39C9FC6E9DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="20490" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
   <si>
     <t>XX.</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Buku </t>
   </si>
   <si>
+    <t>12.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Semua jenjang </t>
   </si>
   <si>
@@ -255,12 +258,10 @@
     <t>SUB BUTIR KEGIATAN</t>
   </si>
   <si>
-    <t>25% AK 
-kenaikan 
-pangkat</t>
-  </si>
-  <si>
-    <t>SUB UNSUR</t>
+    <t>SUB-UNSUR</t>
+  </si>
+  <si>
+    <t>15% AK kenaikan pangkat</t>
   </si>
 </sst>
 </file>
@@ -322,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -459,6 +460,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -466,7 +476,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -570,6 +580,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -609,21 +622,18 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="3" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -633,19 +643,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -933,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA121D6-017A-4F9B-8DEF-C3048D9FCF7B}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,31 +967,31 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="52" t="s">
-        <v>71</v>
+      <c r="D1" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -984,30 +1001,30 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="7" t="s">
+      <c r="A3" s="60"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="60" t="s">
-        <v>76</v>
+      <c r="G3" s="35" t="s">
+        <v>6</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1015,25 +1032,25 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="16"/>
-      <c r="E4" s="9" t="s">
-        <v>7</v>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="36">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>78</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="2"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
+      <c r="D5" s="56" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="27"/>
@@ -1043,19 +1060,19 @@
     <row r="6" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="35"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="20"/>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="37">
+        <v>11</v>
+      </c>
+      <c r="G6" s="38">
         <v>8</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,25 +1080,25 @@
       <c r="B7" s="2"/>
       <c r="C7" s="20"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
+      <c r="E7" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="38">
+        <v>13</v>
+      </c>
+      <c r="G7" s="39">
         <v>4</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="7" t="s">
-        <v>13</v>
+      <c r="C8" s="36"/>
+      <c r="D8" s="56" t="s">
+        <v>14</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="31"/>
@@ -1091,153 +1108,153 @@
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="35"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="37">
+        <v>15</v>
+      </c>
+      <c r="G9" s="38">
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="35"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
+      <c r="E10" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="38">
+        <v>16</v>
+      </c>
+      <c r="G10" s="39">
         <v>4</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="7" t="s">
-        <v>16</v>
+      <c r="C11" s="36"/>
+      <c r="D11" s="56" t="s">
+        <v>17</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="27"/>
-      <c r="G11" s="39"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="20"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="9" t="s">
-        <v>17</v>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="36">
+        <v>15</v>
+      </c>
+      <c r="G12" s="37">
         <v>7</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="35"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="7" t="s">
-        <v>18</v>
+      <c r="E13" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>20</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="7" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="60"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="32" t="s">
+        <v>21</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="41" t="s">
         <v>22</v>
       </c>
+      <c r="G14" s="42" t="s">
+        <v>23</v>
+      </c>
       <c r="H14" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="2"/>
       <c r="C15" s="22"/>
-      <c r="D15" s="9" t="s">
-        <v>23</v>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="E15" s="33"/>
       <c r="F15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="42">
+        <v>22</v>
+      </c>
+      <c r="G15" s="43">
         <v>2.5</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
       <c r="C16" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="59"/>
+      <c r="D16" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="17"/>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="21"/>
       <c r="C17" s="55"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="13">
         <v>7</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1245,45 +1262,45 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="7" t="s">
-        <v>26</v>
+      <c r="E18" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="43">
+        <v>13</v>
+      </c>
+      <c r="G18" s="44">
         <v>3.5</v>
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="7" t="s">
-        <v>27</v>
+      <c r="D19" s="56" t="s">
+        <v>28</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="7" t="s">
-        <v>17</v>
+      <c r="E20" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" s="13">
         <v>3.5</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1291,373 +1308,370 @@
       <c r="B21" s="2"/>
       <c r="C21" s="9"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="7" t="s">
-        <v>28</v>
+      <c r="E21" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G21" s="13">
         <v>1.5</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>32</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G22" s="12">
         <v>8</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="7" t="s">
-        <v>33</v>
+      <c r="C23" s="6"/>
+      <c r="D23" s="56" t="s">
+        <v>34</v>
       </c>
       <c r="E23" s="32"/>
       <c r="F23" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G23" s="13">
         <v>3</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="7" t="s">
         <v>38</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>39</v>
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="44" t="s">
         <v>40</v>
       </c>
+      <c r="G24" s="45" t="s">
+        <v>41</v>
+      </c>
       <c r="H24" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="2"/>
       <c r="C25" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="7" t="s">
         <v>42</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>43</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="39"/>
+      <c r="G25" s="40"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="2"/>
       <c r="C26" s="55"/>
       <c r="D26" s="22"/>
       <c r="E26" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="45">
+        <v>45</v>
+      </c>
+      <c r="G26" s="46">
         <v>3</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="2"/>
       <c r="C27" s="55"/>
       <c r="D27" s="22"/>
       <c r="E27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>45</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>44</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="2"/>
       <c r="C28" s="55"/>
       <c r="D28" s="22"/>
       <c r="E28" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="45">
+        <v>45</v>
+      </c>
+      <c r="G28" s="46">
         <v>1</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="2"/>
       <c r="C29" s="20"/>
-      <c r="D29" s="9" t="s">
-        <v>47</v>
+      <c r="D29" s="56" t="s">
+        <v>48</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="31"/>
-      <c r="G29" s="47"/>
+      <c r="G29" s="48"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="7" t="s">
-        <v>48</v>
+      <c r="C30" s="36"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G30" s="13">
         <v>1.5</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="7" t="s">
+      <c r="D31" s="25"/>
+      <c r="E31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>49</v>
       </c>
       <c r="G31" s="13">
         <v>1</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="2"/>
       <c r="C32" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="7" t="s">
         <v>52</v>
+      </c>
+      <c r="D32" s="56" t="s">
+        <v>53</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="31"/>
-      <c r="G32" s="47"/>
+      <c r="G32" s="48"/>
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
       <c r="B33" s="2"/>
       <c r="C33" s="55"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="7" t="s">
-        <v>53</v>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="45">
+        <v>55</v>
+      </c>
+      <c r="G33" s="46">
         <v>1</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="7" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="45">
+      <c r="G34" s="46">
         <v>0.75</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="57"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="32"/>
       <c r="F35" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G35" s="8">
         <v>0.5</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="2"/>
       <c r="C36" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" s="7" t="s">
         <v>59</v>
+      </c>
+      <c r="D36" s="56" t="s">
+        <v>60</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="31"/>
-      <c r="G36" s="47"/>
+      <c r="G36" s="48"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="2"/>
       <c r="C37" s="55"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="7" t="s">
-        <v>60</v>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G37" s="45">
+        <v>62</v>
+      </c>
+      <c r="G37" s="46">
         <v>3</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="7" t="s">
+      <c r="C38" s="36"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="G38" s="8">
         <v>2</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="2"/>
       <c r="C39" s="20"/>
       <c r="D39" s="50"/>
-      <c r="E39" s="7" t="s">
-        <v>63</v>
+      <c r="E39" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G39" s="23">
         <v>1</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="2"/>
       <c r="C40" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="48" t="s">
         <v>65</v>
+      </c>
+      <c r="D40" s="57" t="s">
+        <v>66</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="27"/>
       <c r="G40" s="49"/>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
       <c r="C41" s="54"/>
       <c r="D41" s="50"/>
-      <c r="E41" s="7" t="s">
-        <v>66</v>
+      <c r="E41" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" s="45">
+        <v>68</v>
+      </c>
+      <c r="G41" s="46">
         <v>4</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="5">
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C22:C23"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D35:E35"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="C32:C33"/>
   </mergeCells>

</xml_diff>